<commit_message>
Format the testcase file
</commit_message>
<xml_diff>
--- a/resources/Testcase_1.0.xlsx
+++ b/resources/Testcase_1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\HDS\qa-assignment\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\HDS\fork-again\qa-assignment-tml\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -269,12 +269,6 @@
   </si>
   <si>
     <t>VMO</t>
-  </si>
-  <si>
-    <t>User Story 1</t>
-  </si>
-  <si>
-    <t>User Story 2</t>
   </si>
   <si>
     <t xml:space="preserve">Environment </t>
@@ -800,6 +794,12 @@
       <t>no image found in zip file"</t>
     </r>
   </si>
+  <si>
+    <t>User Story 1: api/image</t>
+  </si>
+  <si>
+    <t>User Story 2: api/zip</t>
+  </si>
 </sst>
 </file>
 
@@ -809,11 +809,18 @@
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1194,96 +1201,87 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1291,195 +1289,207 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1487,62 +1497,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA8D08D"/>
-          <bgColor rgb="FFA8D08D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1700,6 +1654,62 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFA8D08D"/>
           <bgColor rgb="FFA8D08D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA8D08D"/>
+          <bgColor rgb="FFA8D08D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBE4D5"/>
+          <bgColor rgb="FFFBE4D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4C6E7"/>
+          <bgColor rgb="FFB4C6E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2177,17 +2187,17 @@
   <sheetData>
     <row r="1" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2267,7 +2277,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="90"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="84"/>
       <c r="H4" s="84"/>
       <c r="I4" s="84"/>
@@ -2487,7 +2497,7 @@
     </row>
     <row r="12" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="87" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="84"/>
@@ -2552,7 +2562,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="92" t="s">
+      <c r="I14" s="88" t="s">
         <v>1</v>
       </c>
       <c r="J14" s="84"/>
@@ -2832,17 +2842,17 @@
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="93" t="s">
+      <c r="C24" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="94"/>
-      <c r="E24" s="95" t="s">
+      <c r="D24" s="90"/>
+      <c r="E24" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="94"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -2864,11 +2874,11 @@
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="83" t="s">
+      <c r="C25" s="92" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="84"/>
-      <c r="E25" s="88">
+      <c r="E25" s="83">
         <v>45146</v>
       </c>
       <c r="F25" s="84"/>
@@ -2896,11 +2906,11 @@
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="83" t="s">
+      <c r="C26" s="92" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="84"/>
-      <c r="E26" s="85" t="s">
+      <c r="E26" s="93" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="84"/>
@@ -2928,11 +2938,11 @@
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="92" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="84"/>
-      <c r="E27" s="85" t="s">
+      <c r="E27" s="93" t="s">
         <v>73</v>
       </c>
       <c r="F27" s="84"/>
@@ -2960,11 +2970,11 @@
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="92" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="84"/>
-      <c r="E28" s="85" t="s">
+      <c r="E28" s="93" t="s">
         <v>74</v>
       </c>
       <c r="F28" s="84"/>
@@ -2992,11 +3002,11 @@
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="92" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="84"/>
-      <c r="E29" s="85" t="s">
+      <c r="E29" s="93" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="84"/>
@@ -3286,9 +3296,9 @@
         <v>11</v>
       </c>
       <c r="H39" s="10"/>
-      <c r="I39" s="86"/>
-      <c r="J39" s="87"/>
-      <c r="K39" s="87"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -9724,6 +9734,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="I39:K39"/>
     <mergeCell ref="E25:I25"/>
     <mergeCell ref="B1:J1"/>
@@ -9740,7 +9751,6 @@
     <mergeCell ref="E26:I26"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E24">
@@ -9778,7 +9788,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="94" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="84"/>
@@ -11245,13 +11255,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11286,19 +11293,19 @@
     </row>
     <row r="2" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27"/>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="99"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="97"/>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
@@ -11353,7 +11360,7 @@
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="29" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -11369,7 +11376,7 @@
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="32" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -12770,8 +12777,8 @@
   </sheetPr>
   <dimension ref="A1:Y970"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12826,13 +12833,13 @@
       <c r="A2" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="100" t="s">
-        <v>101</v>
+      <c r="B2" s="104" t="s">
+        <v>99</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="103"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>
@@ -12857,13 +12864,13 @@
       <c r="A3" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="100" t="s">
-        <v>93</v>
+      <c r="B3" s="104" t="s">
+        <v>91</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="103"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
@@ -12888,13 +12895,13 @@
       <c r="A4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="103"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
@@ -12919,13 +12926,13 @@
       <c r="A5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="103"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="44"/>
@@ -12950,13 +12957,13 @@
       <c r="A6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
@@ -13086,46 +13093,46 @@
       <c r="Y9" s="44"/>
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="106" t="s">
+      <c r="F10" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="106" t="s">
+      <c r="H10" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="107" t="s">
+      <c r="I10" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="106" t="s">
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="106" t="s">
+      <c r="N10" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="O10" s="106" t="s">
+      <c r="O10" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="106" t="s">
+      <c r="P10" s="100" t="s">
         <v>63</v>
       </c>
       <c r="Q10" s="54"/>
@@ -13139,14 +13146,14 @@
       <c r="Y10" s="54"/>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="105"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="55" t="s">
         <v>64</v>
       </c>
@@ -13159,10 +13166,10 @@
       <c r="L11" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="99"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="99"/>
       <c r="Q11" s="56"/>
       <c r="R11" s="56"/>
       <c r="S11" s="56"/>
@@ -13174,7 +13181,7 @@
       <c r="Y11" s="56"/>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="75" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="60"/>
@@ -13203,28 +13210,28 @@
       <c r="Y12" s="44"/>
     </row>
     <row r="13" spans="1:25" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
-        <v>94</v>
+      <c r="A13" s="79" t="s">
+        <v>92</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="76" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="76" t="s">
-        <v>99</v>
+      <c r="F13" s="74" t="s">
+        <v>97</v>
       </c>
       <c r="G13" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I13" s="59"/>
@@ -13233,7 +13240,7 @@
       <c r="L13" s="58"/>
       <c r="M13" s="59"/>
       <c r="N13" s="64"/>
-      <c r="O13" s="80" t="s">
+      <c r="O13" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P13" s="65"/>
@@ -13248,28 +13255,28 @@
       <c r="Y13" s="44"/>
     </row>
     <row r="14" spans="1:25" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="79" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="D14" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="76" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="76" t="s">
-        <v>128</v>
+      <c r="F14" s="74" t="s">
+        <v>126</v>
       </c>
       <c r="G14" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="59"/>
@@ -13278,7 +13285,7 @@
       <c r="L14" s="58"/>
       <c r="M14" s="59"/>
       <c r="N14" s="64"/>
-      <c r="O14" s="80" t="s">
+      <c r="O14" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P14" s="65"/>
@@ -13292,27 +13299,27 @@
       <c r="X14" s="44"/>
       <c r="Y14" s="44"/>
     </row>
-    <row r="15" spans="1:25" s="82" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="81" t="s">
+    <row r="15" spans="1:25" s="80" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="D15" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="E15" s="74"/>
+      <c r="F15" s="74" t="s">
         <v>115</v>
-      </c>
-      <c r="D15" s="78" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76" t="s">
-        <v>117</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I15" s="59"/>
@@ -13321,7 +13328,7 @@
       <c r="L15" s="58"/>
       <c r="M15" s="59"/>
       <c r="N15" s="64"/>
-      <c r="O15" s="80" t="s">
+      <c r="O15" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P15" s="65"/>
@@ -20954,6 +20961,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="O10:O11"/>
@@ -20967,11 +20979,6 @@
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="H13">
     <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
@@ -21069,37 +21076,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"API"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"Functionality"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:L15">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(K15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J15">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:L15">
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(I15))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(L15))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21189,13 +21196,13 @@
       <c r="A2" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="100" t="s">
-        <v>101</v>
+      <c r="B2" s="104" t="s">
+        <v>99</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="103"/>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>
@@ -21220,13 +21227,13 @@
       <c r="A3" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="100" t="s">
-        <v>93</v>
+      <c r="B3" s="104" t="s">
+        <v>91</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="103"/>
       <c r="G3" s="44"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
@@ -21251,13 +21258,13 @@
       <c r="A4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="103"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
@@ -21282,13 +21289,13 @@
       <c r="A5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="101"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="103"/>
       <c r="G5" s="44"/>
       <c r="H5" s="44"/>
       <c r="I5" s="44"/>
@@ -21313,13 +21320,13 @@
       <c r="A6" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="44"/>
       <c r="H6" s="44"/>
       <c r="I6" s="44"/>
@@ -21449,46 +21456,46 @@
       <c r="Y9" s="44"/>
     </row>
     <row r="10" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="106" t="s">
+      <c r="F10" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="106" t="s">
+      <c r="H10" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="107" t="s">
+      <c r="I10" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="102"/>
-      <c r="M10" s="106" t="s">
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="106" t="s">
+      <c r="N10" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="O10" s="106" t="s">
+      <c r="O10" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="106" t="s">
+      <c r="P10" s="100" t="s">
         <v>63</v>
       </c>
       <c r="Q10" s="54"/>
@@ -21502,14 +21509,14 @@
       <c r="Y10" s="54"/>
     </row>
     <row r="11" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="105"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="55" t="s">
         <v>64</v>
       </c>
@@ -21522,10 +21529,10 @@
       <c r="L11" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
+      <c r="M11" s="99"/>
+      <c r="N11" s="99"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="99"/>
       <c r="Q11" s="56"/>
       <c r="R11" s="56"/>
       <c r="S11" s="56"/>
@@ -21537,7 +21544,7 @@
       <c r="Y11" s="56"/>
     </row>
     <row r="12" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="75" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="60"/>
@@ -21566,28 +21573,28 @@
       <c r="Y12" s="44"/>
     </row>
     <row r="13" spans="1:25" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
-        <v>94</v>
+      <c r="A13" s="79" t="s">
+        <v>92</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="E13" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="78" t="s">
+      <c r="F13" s="74" t="s">
         <v>120</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="76" t="s">
-        <v>122</v>
       </c>
       <c r="G13" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I13" s="59"/>
@@ -21596,7 +21603,7 @@
       <c r="L13" s="58"/>
       <c r="M13" s="59"/>
       <c r="N13" s="64"/>
-      <c r="O13" s="80" t="s">
+      <c r="O13" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P13" s="65"/>
@@ -21611,28 +21618,28 @@
       <c r="Y13" s="44"/>
     </row>
     <row r="14" spans="1:25" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="81" t="s">
-        <v>95</v>
+      <c r="A14" s="79" t="s">
+        <v>93</v>
       </c>
-      <c r="B14" s="75" t="s">
-        <v>123</v>
+      <c r="B14" s="73" t="s">
+        <v>121</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="78" t="s">
-        <v>126</v>
+      <c r="E14" s="74" t="s">
+        <v>96</v>
       </c>
-      <c r="E14" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="76" t="s">
-        <v>127</v>
+      <c r="F14" s="74" t="s">
+        <v>125</v>
       </c>
       <c r="G14" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="59"/>
@@ -21641,7 +21648,7 @@
       <c r="L14" s="58"/>
       <c r="M14" s="59"/>
       <c r="N14" s="64"/>
-      <c r="O14" s="80" t="s">
+      <c r="O14" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P14" s="65"/>
@@ -21655,29 +21662,29 @@
       <c r="X14" s="44"/>
       <c r="Y14" s="44"/>
     </row>
-    <row r="15" spans="1:25" s="82" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="81" t="s">
-        <v>113</v>
+    <row r="15" spans="1:25" s="80" customFormat="1" ht="198" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="79" t="s">
+        <v>111</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="76" t="s">
+      <c r="E15" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="F15" s="74" t="s">
         <v>131</v>
-      </c>
-      <c r="E15" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="76" t="s">
-        <v>133</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="77" t="s">
         <v>70</v>
       </c>
       <c r="I15" s="59"/>
@@ -21686,7 +21693,7 @@
       <c r="L15" s="58"/>
       <c r="M15" s="59"/>
       <c r="N15" s="64"/>
-      <c r="O15" s="80" t="s">
+      <c r="O15" s="78" t="s">
         <v>73</v>
       </c>
       <c r="P15" s="65"/>
@@ -29319,6 +29326,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="F10:F11"/>
@@ -29327,109 +29344,99 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="N10:N11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="32" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="15" operator="equal">
       <formula>"API"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="31" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
       <formula>"Functionality"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="30" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J12 K12:L13">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:J13">
-    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:K3 I5:K5 I6:L9 I11:L11">
-    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:K4">
-    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(I4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:L3 I5:L9 I11:L11">
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:L4">
-    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:L13">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(I12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L5">
-    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="14" priority="26" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(L13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"API"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"Functionality"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"UI"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:L14">
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(K14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(I14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:L14">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(I14))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="7" priority="14" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(L14))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29496,7 +29503,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -29512,28 +29519,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="D1" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="70" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="70" t="s">
-        <v>80</v>
-      </c>
       <c r="E1" s="70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F1" s="70" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" s="70" t="s">
         <v>58</v>
       </c>
       <c r="H1" s="70" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I1" s="70" t="s">
         <v>63</v>
@@ -29541,79 +29548,79 @@
     </row>
     <row r="2" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
-      <c r="B2" s="73" t="s">
-        <v>102</v>
+      <c r="B2" s="108" t="s">
+        <v>100</v>
       </c>
-      <c r="C2" s="69" t="s">
-        <v>84</v>
+      <c r="C2" s="107" t="s">
+        <v>82</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
-      <c r="E2" s="74" t="s">
-        <v>89</v>
+      <c r="E2" s="106" t="s">
+        <v>87</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G2" s="69" t="s">
         <v>70</v>
       </c>
       <c r="H2" s="71"/>
       <c r="I2" s="69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A3" s="71"/>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="108" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="E3" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>106</v>
-      </c>
       <c r="F3" s="71" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G3" s="71" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H3" s="71"/>
       <c r="I3" s="71" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="185.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="71"/>
+      <c r="B4" s="108" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="71" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="185.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
-      <c r="B4" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="69" t="s">
+      <c r="F4" s="69" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="69" t="s">
-        <v>87</v>
       </c>
       <c r="G4" s="69" t="s">
         <v>70</v>
       </c>
       <c r="H4" s="71"/>
       <c r="I4" s="71" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>